<commit_message>
create record of all invoices
</commit_message>
<xml_diff>
--- a/poslogs_file.xlsx
+++ b/poslogs_file.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="237">
   <si>
     <t>Inv-S.NO</t>
   </si>
@@ -55,121 +55,673 @@
     <t>InvCaseCost</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>011210000018</t>
+  </si>
+  <si>
+    <t>DEEP SPI CORIANDER SEEDS7OZ (20)</t>
+  </si>
+  <si>
+    <t>TABASCO PEPPER SAUCE  Apna</t>
+  </si>
+  <si>
+    <t>CAS S53</t>
+  </si>
+  <si>
+    <t>0.88</t>
+  </si>
+  <si>
+    <t>1.99</t>
+  </si>
+  <si>
+    <t>2.09</t>
+  </si>
+  <si>
+    <t>126.14</t>
+  </si>
+  <si>
+    <t>137.50</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>17.69</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>011433073165</t>
+  </si>
+  <si>
+    <t>DEEP SPI CARDAMOM PWD 3 5OZ (20)</t>
+  </si>
+  <si>
+    <t>DEEP CUMIN POWDER</t>
+  </si>
+  <si>
+    <t>CAS S125</t>
+  </si>
+  <si>
+    <t>26.01</t>
+  </si>
+  <si>
+    <t>1.9</t>
+  </si>
+  <si>
+    <t>33.81</t>
+  </si>
+  <si>
+    <t>-92.70</t>
+  </si>
+  <si>
+    <t>29.99</t>
+  </si>
+  <si>
+    <t>130.04</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>011433071185</t>
+  </si>
+  <si>
+    <t>DEEP SPI COR-CUMIN PWD 14OZ (20)</t>
+  </si>
+  <si>
+    <t>DEEP CORIANDER CUMIN POWDER</t>
+  </si>
+  <si>
+    <t>CAS S18</t>
+  </si>
+  <si>
+    <t>3.68</t>
+  </si>
+  <si>
+    <t>3.99</t>
+  </si>
+  <si>
+    <t>4.78</t>
+  </si>
+  <si>
+    <t>8.42</t>
+  </si>
+  <si>
+    <t>29.89</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>44.19</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>011433073141</t>
+  </si>
+  <si>
+    <t>DEEP SPI CORIANDERPWDER7OZ (20)</t>
+  </si>
+  <si>
+    <t>DEEP CORRIANDER POWDER</t>
+  </si>
+  <si>
+    <t>CAS S54</t>
+  </si>
+  <si>
+    <t>1.14</t>
+  </si>
+  <si>
+    <t>29.55</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>011433021111</t>
+  </si>
+  <si>
+    <t>DEEP SPI CLOVE 7OZ (20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEEP HOT MIX ORIGINAL  </t>
+  </si>
+  <si>
+    <t>CAS S39N</t>
+  </si>
+  <si>
+    <t>11.71</t>
+  </si>
+  <si>
+    <t>15.22</t>
+  </si>
+  <si>
+    <t>-65.93</t>
+  </si>
+  <si>
+    <t>29.97</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>93.69</t>
+  </si>
+  <si>
+    <t>tabasco pepper sauc</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>011433134446</t>
+  </si>
+  <si>
+    <t>DEEP SPI CINNAMON STICK 7OZ (20)</t>
+  </si>
+  <si>
+    <t>DEEP CINNAMON STICKS</t>
+  </si>
+  <si>
+    <t>CAS S157L</t>
+  </si>
+  <si>
+    <t>2.48</t>
+  </si>
+  <si>
+    <t>3.79</t>
+  </si>
+  <si>
+    <t>2.64</t>
+  </si>
+  <si>
+    <t>52.82</t>
+  </si>
+  <si>
+    <t>89.39</t>
+  </si>
+  <si>
+    <t>52.89</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>011433071130</t>
+  </si>
+  <si>
+    <t>DEEP SPI CORIANDERSEEDSL4OZ( (20)</t>
+  </si>
+  <si>
+    <t>DEEP CORIANDER SEEDS</t>
+  </si>
+  <si>
+    <t>CAS S13</t>
+  </si>
+  <si>
+    <t>1.65</t>
+  </si>
+  <si>
+    <t>2.15</t>
+  </si>
+  <si>
+    <t>141.82</t>
+  </si>
+  <si>
+    <t>30.30</t>
+  </si>
+  <si>
+    <t>32.98</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>011433134316</t>
+  </si>
+  <si>
+    <t>DEEP SPI CUMIN SEEDS 14OZ (20)</t>
+  </si>
+  <si>
+    <t>DEEP CUMIN SEEDS</t>
+  </si>
+  <si>
+    <t>CAS S15</t>
+  </si>
+  <si>
+    <t>2.49</t>
+  </si>
+  <si>
+    <t>4.49</t>
+  </si>
+  <si>
+    <t>3.24</t>
+  </si>
+  <si>
+    <t>80.32</t>
+  </si>
+  <si>
+    <t>30.12</t>
+  </si>
+  <si>
+    <t>49.79</t>
+  </si>
+  <si>
+    <t>714760810662</t>
+  </si>
+  <si>
+    <t>DEEP SPI CORIANDERPDR14OZ (20)</t>
+  </si>
+  <si>
+    <t>DEER CORIANDER POWDER - CAS S14</t>
+  </si>
+  <si>
+    <t>CAS S14</t>
+  </si>
+  <si>
+    <t>1.8</t>
+  </si>
+  <si>
+    <t>2.99</t>
+  </si>
+  <si>
+    <t>1.55</t>
+  </si>
+  <si>
+    <t>66.11</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>30.99</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>011433073158</t>
+  </si>
+  <si>
+    <t>DEEP SPI CUMIN SEEDS 7OZ (20)</t>
+  </si>
+  <si>
+    <t>CAS S55</t>
+  </si>
+  <si>
+    <t>1.32</t>
+  </si>
+  <si>
+    <t>1.72</t>
+  </si>
+  <si>
+    <t>88.64</t>
+  </si>
+  <si>
+    <t>26.49</t>
+  </si>
+  <si>
+    <t>DEEP SPI CUMINPOWDER7OZ (20)</t>
+  </si>
+  <si>
+    <t>CAS S56</t>
+  </si>
+  <si>
+    <t>1.66</t>
+  </si>
+  <si>
+    <t>2.16</t>
+  </si>
+  <si>
+    <t>50.00</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>011433134323</t>
+  </si>
+  <si>
+    <t>DEEP SPI CUMIN PWD 14OZ (20)</t>
+  </si>
+  <si>
+    <t>CAS S16</t>
+  </si>
+  <si>
+    <t>3.04</t>
+  </si>
+  <si>
+    <t>5.49</t>
+  </si>
+  <si>
+    <t>2.65</t>
+  </si>
+  <si>
+    <t>3.44</t>
+  </si>
+  <si>
+    <t>80.59</t>
+  </si>
+  <si>
+    <t>29.81</t>
+  </si>
+  <si>
+    <t>52.99</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>011433112703</t>
+  </si>
+  <si>
+    <t>DEEP SPI DILL SEEDS 7 OZ (20)</t>
+  </si>
+  <si>
+    <t>DEEP DILL SEEDS</t>
+  </si>
+  <si>
+    <t>CAS S81</t>
+  </si>
+  <si>
+    <t>0.99</t>
+  </si>
+  <si>
+    <t>1.29</t>
+  </si>
+  <si>
+    <t>202.02</t>
+  </si>
+  <si>
+    <t>19.89</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>011433111782</t>
+  </si>
+  <si>
+    <t>DEEP SPI FENNLSEEDSALTDL4OZ (20)</t>
+  </si>
+  <si>
+    <t>DEEP SALTED FENNEL SEEDS</t>
+  </si>
+  <si>
+    <t>CAS S26</t>
+  </si>
+  <si>
+    <t>52.21</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>011433114493</t>
+  </si>
+  <si>
+    <t>DEEP SPI EDIBLE GUM 3 5OZ (20)</t>
+  </si>
+  <si>
+    <t>DEEP EDIBLE GUM</t>
+  </si>
+  <si>
+    <t>CAS S106</t>
+  </si>
+  <si>
+    <t>1.30</t>
+  </si>
+  <si>
+    <t>1.69</t>
+  </si>
+  <si>
+    <t>130.00</t>
+  </si>
+  <si>
+    <t>30.00</t>
+  </si>
+  <si>
+    <t>26.05</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>011433071178</t>
+  </si>
+  <si>
+    <t>DEEP SPI FENNEL SEEDS 14OZ (20)</t>
+  </si>
+  <si>
+    <t>DEEP FENEL SEEDS</t>
+  </si>
+  <si>
+    <t>CAS S17</t>
+  </si>
+  <si>
+    <t>2.59</t>
+  </si>
+  <si>
+    <t>100.50</t>
+  </si>
+  <si>
+    <t>30.15</t>
+  </si>
+  <si>
+    <t>39.79</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>011433114462</t>
+  </si>
+  <si>
+    <t>DEEP SPI GARAM MASALA 7OZ (20)</t>
+  </si>
+  <si>
+    <t>DEEP GARAM MASALA WHOLE</t>
+  </si>
+  <si>
+    <t>CAS S65</t>
+  </si>
+  <si>
+    <t>1.98</t>
+  </si>
+  <si>
+    <t>1.75</t>
+  </si>
+  <si>
+    <t>2.27</t>
+  </si>
+  <si>
+    <t>51.01</t>
+  </si>
+  <si>
+    <t>29.71</t>
+  </si>
+  <si>
+    <t>35.09</t>
+  </si>
+  <si>
+    <t>011433116008</t>
+  </si>
+  <si>
+    <t>DEEP SPI FENNEL PWD 7OZ (20)</t>
+  </si>
+  <si>
+    <t>DEEP METHI BHARDO  Apna</t>
+  </si>
+  <si>
+    <t>CAS S124</t>
+  </si>
+  <si>
+    <t>1.93</t>
+  </si>
+  <si>
+    <t>2.51</t>
+  </si>
+  <si>
+    <t>54.92</t>
+  </si>
+  <si>
+    <t>30.05</t>
+  </si>
+  <si>
+    <t>30.84</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>DEEP SPI CURRYPOWDER7OZ (20)</t>
+  </si>
+  <si>
+    <t>CAS S68</t>
+  </si>
+  <si>
+    <t>1.47</t>
+  </si>
+  <si>
+    <t>1.91</t>
+  </si>
+  <si>
+    <t>69.39</t>
+  </si>
+  <si>
+    <t>29.93</t>
+  </si>
+  <si>
     <t>19</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>8901063151505</t>
-  </si>
-  <si>
-    <t>BRITANNI MILKBIKIS CREAM3. 5 (48)</t>
-  </si>
-  <si>
-    <t>BRITANNIA  MILK BIKIS</t>
-  </si>
-  <si>
-    <t>CAS BN109</t>
-  </si>
-  <si>
-    <t>0.45</t>
-  </si>
-  <si>
-    <t>0.79</t>
+    <t>011433073196</t>
+  </si>
+  <si>
+    <t>DEEP SPI FENUGREEK SEEDS7OZ (20)</t>
+  </si>
+  <si>
+    <t>DEEP FENUGREEK SEEDS</t>
+  </si>
+  <si>
+    <t>CAS S59</t>
+  </si>
+  <si>
+    <t>0.66</t>
+  </si>
+  <si>
+    <t>1.49</t>
+  </si>
+  <si>
+    <t>0.86</t>
+  </si>
+  <si>
+    <t>125.76</t>
+  </si>
+  <si>
+    <t>13.29</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>011433160735</t>
+  </si>
+  <si>
+    <t>DEEP SPI KSHMIRICHILIPDL4OZ (20)</t>
+  </si>
+  <si>
+    <t>DEEP RED CHILLI KASHMIRI</t>
+  </si>
+  <si>
+    <t>CAS S167</t>
+  </si>
+  <si>
+    <t>2.76</t>
+  </si>
+  <si>
+    <t>3.59</t>
+  </si>
+  <si>
+    <t>62.68</t>
+  </si>
+  <si>
+    <t>30.07</t>
+  </si>
+  <si>
+    <t>55.18</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>011433160742</t>
+  </si>
+  <si>
+    <t>DEEP SPI KSHMIRICHILIPD28OZ (10)</t>
+  </si>
+  <si>
+    <t>DEEP RED CHILLI POWDER KASHMIRI</t>
+  </si>
+  <si>
+    <t>CAS S168</t>
+  </si>
+  <si>
+    <t>5.52</t>
+  </si>
+  <si>
+    <t>6.99</t>
+  </si>
+  <si>
+    <t>7.18</t>
+  </si>
+  <si>
+    <t>26.63</t>
+  </si>
+  <si>
+    <t>011433071192</t>
+  </si>
+  <si>
+    <t>DEEP SPI FENUGREEKSEEDS14OZ (20)</t>
+  </si>
+  <si>
+    <t>CAS S19</t>
+  </si>
+  <si>
+    <t>1.28</t>
   </si>
   <si>
     <t>2.79</t>
   </si>
   <si>
-    <t>75.56</t>
-  </si>
-  <si>
-    <t>520.00</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>21.70</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>011433158220</t>
-  </si>
-  <si>
-    <t>DEEP FLO CRACKWHEAT (KANSAR) (10)</t>
-  </si>
-  <si>
-    <t>DEEP FADA(KANSAR) SMALL 3</t>
-  </si>
-  <si>
-    <t>CAS F73</t>
-  </si>
-  <si>
-    <t>4.49</t>
-  </si>
-  <si>
-    <t>5.49</t>
-  </si>
-  <si>
-    <t>60.93</t>
-  </si>
-  <si>
-    <t>96.77</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>27.90</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>011433158725</t>
-  </si>
-  <si>
-    <t>DEEP FLO BHAKRI FLOUR 81B (5)</t>
-  </si>
-  <si>
-    <t>DEEP BHAKRI FLOUR</t>
-  </si>
-  <si>
-    <t>CAS F65</t>
-  </si>
-  <si>
-    <t>6.08</t>
-  </si>
-  <si>
-    <t>7.79</t>
-  </si>
-  <si>
-    <t>6.79</t>
-  </si>
-  <si>
-    <t>28.13</t>
-  </si>
-  <si>
-    <t>11.68</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>30.40</t>
+    <t>117.97</t>
+  </si>
+  <si>
+    <t>29.69</t>
+  </si>
+  <si>
+    <t>25.59</t>
   </si>
   <si>
     <t>VENDOR:chetak</t>
   </si>
   <si>
-    <t>INV #:997391 - INV DATE:2022-02-02</t>
-  </si>
-  <si>
-    <t>LINKED BY #:deeepanshunayak</t>
+    <t>INV #:test 1 - INV DATE:2022-04-28</t>
+  </si>
+  <si>
+    <t>LINKED BY #:jigyasubisht7</t>
   </si>
 </sst>
 </file>
@@ -590,7 +1142,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N31"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="10" customWidth="1"/>
@@ -711,25 +1263,25 @@
         <v>31</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="H3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="J3" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>37</v>
@@ -779,19 +1331,943 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="D5" s="4" t="s">
         <v>52</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>